<commit_message>
Fix alternate colors for subjects
Co-authored-by: Zak Auerbach <zak@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/san_joaquin.xlsx
+++ b/test_fixtures/san_joaquin.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
-  <workbookPr date1904="1" codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/san_joaquin/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753E4C28-DBF8-4744-AA19-1AC5B74D6AA0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
+  <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="213">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -656,12 +655,15 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="000000000000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -968,7 +970,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2119,18 +2121,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:IW43"/>
+  <dimension ref="A1:IW43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection activeCell="O54" sqref="O54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
@@ -2234,7 +2235,7 @@
     <col min="109" max="257" width="8.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:108" s="33" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:108" s="33" customFormat="1" ht="27.75" customHeight="1">
       <c r="B1" s="30"/>
       <c r="C1" s="31"/>
       <c r="D1" s="32"/>
@@ -2407,7 +2408,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="2:108" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:108" ht="27.75" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2730,7 +2731,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="2:108" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:108" ht="20.25" customHeight="1">
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5">
@@ -2865,7 +2866,7 @@
       <c r="DC3" s="6"/>
       <c r="DD3" s="6"/>
     </row>
-    <row r="4" spans="2:108" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:108" ht="20.25" customHeight="1">
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
       <c r="D4" s="10">
@@ -3010,7 +3011,7 @@
       <c r="DC4" s="11"/>
       <c r="DD4" s="11"/>
     </row>
-    <row r="5" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:108" ht="20" customHeight="1">
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
       <c r="D5" s="10">
@@ -3145,7 +3146,7 @@
       <c r="DC5" s="11"/>
       <c r="DD5" s="11"/>
     </row>
-    <row r="6" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:108" ht="20" customHeight="1">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
       <c r="D6" s="10">
@@ -3310,7 +3311,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:108" ht="20" customHeight="1">
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
       <c r="D7" s="10">
@@ -3445,7 +3446,7 @@
       <c r="DC7" s="11"/>
       <c r="DD7" s="11"/>
     </row>
-    <row r="8" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:108" ht="20" customHeight="1">
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
       <c r="D8" s="10">
@@ -3582,7 +3583,7 @@
       <c r="DC8" s="11"/>
       <c r="DD8" s="11"/>
     </row>
-    <row r="9" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:108" ht="20" customHeight="1">
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
       <c r="D9" s="10">
@@ -3749,7 +3750,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:108" ht="20" customHeight="1">
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
       <c r="D10" s="10">
@@ -3914,7 +3915,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:108" ht="20" customHeight="1">
       <c r="B11" s="13"/>
       <c r="C11" s="14"/>
       <c r="D11" s="15">
@@ -4049,7 +4050,7 @@
       <c r="DC11" s="16"/>
       <c r="DD11" s="16"/>
     </row>
-    <row r="12" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:108" ht="20" customHeight="1">
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
       <c r="D12" s="15">
@@ -4218,7 +4219,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:108" ht="20" customHeight="1">
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
       <c r="D13" s="15">
@@ -4349,7 +4350,10 @@
       <c r="DC13" s="16"/>
       <c r="DD13" s="16"/>
     </row>
-    <row r="14" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:108" ht="20" customHeight="1">
+      <c r="A14" t="s">
+        <v>212</v>
+      </c>
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
       <c r="D14" s="15">
@@ -4518,7 +4522,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:108" ht="20" customHeight="1">
       <c r="B15" s="13"/>
       <c r="C15" s="14"/>
       <c r="D15" s="15">
@@ -4657,7 +4661,7 @@
       <c r="DC15" s="16"/>
       <c r="DD15" s="16"/>
     </row>
-    <row r="16" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:108" ht="20" customHeight="1">
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="10">
@@ -4824,7 +4828,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:108" ht="20" customHeight="1">
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="10">
@@ -4967,7 +4971,7 @@
       <c r="DC17" s="11"/>
       <c r="DD17" s="11"/>
     </row>
-    <row r="18" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:108" ht="20" customHeight="1">
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
       <c r="D18" s="10">
@@ -5110,7 +5114,7 @@
       <c r="DC18" s="11"/>
       <c r="DD18" s="11"/>
     </row>
-    <row r="19" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:108" ht="20" customHeight="1">
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
       <c r="D19" s="10">
@@ -5275,7 +5279,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:108" ht="20" customHeight="1">
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
       <c r="D20" s="10">
@@ -5416,7 +5420,7 @@
       <c r="DC20" s="11"/>
       <c r="DD20" s="11"/>
     </row>
-    <row r="21" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:108" ht="20" customHeight="1">
       <c r="B21" s="13"/>
       <c r="C21" s="14"/>
       <c r="D21" s="15">
@@ -5581,7 +5585,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:108" ht="20" customHeight="1">
       <c r="B22" s="13"/>
       <c r="C22" s="14"/>
       <c r="D22" s="15">
@@ -5724,7 +5728,7 @@
       <c r="DC22" s="16"/>
       <c r="DD22" s="16"/>
     </row>
-    <row r="23" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:108" ht="20" customHeight="1">
       <c r="B23" s="13"/>
       <c r="C23" s="14"/>
       <c r="D23" s="15">
@@ -5889,7 +5893,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:108" ht="20" customHeight="1">
       <c r="B24" s="13"/>
       <c r="C24" s="14"/>
       <c r="D24" s="15">
@@ -6024,7 +6028,7 @@
       <c r="DC24" s="16"/>
       <c r="DD24" s="16"/>
     </row>
-    <row r="25" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:108" ht="20" customHeight="1">
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
       <c r="D25" s="10">
@@ -6167,7 +6171,7 @@
       <c r="DC25" s="11"/>
       <c r="DD25" s="11"/>
     </row>
-    <row r="26" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:108" ht="20" customHeight="1">
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
       <c r="D26" s="10">
@@ -6332,7 +6336,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:108" ht="20" customHeight="1">
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
       <c r="D27" s="10">
@@ -6475,7 +6479,7 @@
       <c r="DC27" s="11"/>
       <c r="DD27" s="11"/>
     </row>
-    <row r="28" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:108" ht="20" customHeight="1">
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10">
@@ -6614,7 +6618,7 @@
       <c r="DC28" s="11"/>
       <c r="DD28" s="11"/>
     </row>
-    <row r="29" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:108" ht="20" customHeight="1">
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
       <c r="D29" s="10">
@@ -6775,7 +6779,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:108" ht="20" customHeight="1">
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10">
@@ -6936,7 +6940,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:108" ht="20" customHeight="1">
       <c r="B31" s="13"/>
       <c r="C31" s="14"/>
       <c r="D31" s="15">
@@ -7101,7 +7105,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:108" ht="20" customHeight="1">
       <c r="B32" s="13"/>
       <c r="C32" s="14"/>
       <c r="D32" s="15">
@@ -7244,7 +7248,7 @@
       <c r="DC32" s="16"/>
       <c r="DD32" s="16"/>
     </row>
-    <row r="33" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:108" ht="20" customHeight="1">
       <c r="B33" s="13"/>
       <c r="C33" s="14"/>
       <c r="D33" s="15">
@@ -7409,1519 +7413,1519 @@
         <v>182</v>
       </c>
     </row>
-    <row r="34" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="15">
+    <row r="34" spans="2:108" ht="20" customHeight="1">
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20">
         <v>95875321</v>
       </c>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="17" t="s">
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="N34" s="17" t="s">
+      <c r="N34" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="O34" s="16"/>
-      <c r="P34" s="15">
+      <c r="O34" s="21"/>
+      <c r="P34" s="20">
         <v>19690514</v>
       </c>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="16"/>
-      <c r="T34" s="16"/>
-      <c r="U34" s="16"/>
-      <c r="V34" s="16"/>
-      <c r="W34" s="16"/>
-      <c r="X34" s="16"/>
-      <c r="Y34" s="16"/>
-      <c r="Z34" s="16"/>
-      <c r="AA34" s="16"/>
-      <c r="AB34" s="16"/>
-      <c r="AC34" s="16"/>
-      <c r="AD34" s="16"/>
-      <c r="AE34" s="16"/>
-      <c r="AF34" s="16"/>
-      <c r="AG34" s="16"/>
-      <c r="AH34" s="16"/>
-      <c r="AI34" s="16"/>
-      <c r="AJ34" s="16"/>
-      <c r="AK34" s="16"/>
-      <c r="AL34" s="16"/>
-      <c r="AM34" s="16"/>
-      <c r="AN34" s="16"/>
-      <c r="AO34" s="16"/>
-      <c r="AP34" s="15">
+      <c r="Q34" s="21"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="21"/>
+      <c r="T34" s="21"/>
+      <c r="U34" s="21"/>
+      <c r="V34" s="21"/>
+      <c r="W34" s="21"/>
+      <c r="X34" s="21"/>
+      <c r="Y34" s="21"/>
+      <c r="Z34" s="21"/>
+      <c r="AA34" s="21"/>
+      <c r="AB34" s="21"/>
+      <c r="AC34" s="21"/>
+      <c r="AD34" s="21"/>
+      <c r="AE34" s="21"/>
+      <c r="AF34" s="21"/>
+      <c r="AG34" s="21"/>
+      <c r="AH34" s="21"/>
+      <c r="AI34" s="21"/>
+      <c r="AJ34" s="21"/>
+      <c r="AK34" s="21"/>
+      <c r="AL34" s="21"/>
+      <c r="AM34" s="21"/>
+      <c r="AN34" s="21"/>
+      <c r="AO34" s="21"/>
+      <c r="AP34" s="20">
         <v>19910411</v>
       </c>
-      <c r="AQ34" s="16"/>
-      <c r="AR34" s="17" t="s">
+      <c r="AQ34" s="21"/>
+      <c r="AR34" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="AS34" s="16"/>
-      <c r="AT34" s="16"/>
-      <c r="AU34" s="16"/>
-      <c r="AV34" s="16"/>
-      <c r="AW34" s="16"/>
-      <c r="AX34" s="17" t="s">
+      <c r="AS34" s="21"/>
+      <c r="AT34" s="21"/>
+      <c r="AU34" s="21"/>
+      <c r="AV34" s="21"/>
+      <c r="AW34" s="21"/>
+      <c r="AX34" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AY34" s="16"/>
-      <c r="AZ34" s="25">
+      <c r="AY34" s="21"/>
+      <c r="AZ34" s="26">
         <v>101001028000</v>
       </c>
-      <c r="BA34" s="16"/>
-      <c r="BB34" s="16"/>
-      <c r="BC34" s="16"/>
-      <c r="BD34" s="17" t="s">
+      <c r="BA34" s="21"/>
+      <c r="BB34" s="21"/>
+      <c r="BC34" s="21"/>
+      <c r="BD34" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="BE34" s="17" t="s">
+      <c r="BE34" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="BF34" s="17" t="s">
+      <c r="BF34" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="BG34" s="16"/>
-      <c r="BH34" s="16"/>
-      <c r="BI34" s="16"/>
-      <c r="BJ34" s="16"/>
-      <c r="BK34" s="16"/>
-      <c r="BL34" s="16"/>
-      <c r="BM34" s="16"/>
-      <c r="BN34" s="16"/>
-      <c r="BO34" s="16"/>
-      <c r="BP34" s="16"/>
-      <c r="BQ34" s="16"/>
-      <c r="BR34" s="16"/>
-      <c r="BS34" s="16"/>
-      <c r="BT34" s="16"/>
-      <c r="BU34" s="16"/>
-      <c r="BV34" s="16"/>
-      <c r="BW34" s="16"/>
-      <c r="BX34" s="16"/>
-      <c r="BY34" s="16"/>
-      <c r="BZ34" s="16"/>
-      <c r="CA34" s="16"/>
-      <c r="CB34" s="16"/>
-      <c r="CC34" s="16"/>
-      <c r="CD34" s="17" t="s">
+      <c r="BG34" s="21"/>
+      <c r="BH34" s="21"/>
+      <c r="BI34" s="21"/>
+      <c r="BJ34" s="21"/>
+      <c r="BK34" s="21"/>
+      <c r="BL34" s="21"/>
+      <c r="BM34" s="21"/>
+      <c r="BN34" s="21"/>
+      <c r="BO34" s="21"/>
+      <c r="BP34" s="21"/>
+      <c r="BQ34" s="21"/>
+      <c r="BR34" s="21"/>
+      <c r="BS34" s="21"/>
+      <c r="BT34" s="21"/>
+      <c r="BU34" s="21"/>
+      <c r="BV34" s="21"/>
+      <c r="BW34" s="21"/>
+      <c r="BX34" s="21"/>
+      <c r="BY34" s="21"/>
+      <c r="BZ34" s="21"/>
+      <c r="CA34" s="21"/>
+      <c r="CB34" s="21"/>
+      <c r="CC34" s="21"/>
+      <c r="CD34" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="CE34" s="17" t="s">
+      <c r="CE34" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="CF34" s="17" t="s">
+      <c r="CF34" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="CG34" s="16"/>
-      <c r="CH34" s="16"/>
-      <c r="CI34" s="16"/>
-      <c r="CJ34" s="17" t="s">
+      <c r="CG34" s="21"/>
+      <c r="CH34" s="21"/>
+      <c r="CI34" s="21"/>
+      <c r="CJ34" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="CK34" s="15">
+      <c r="CK34" s="20">
         <v>6</v>
       </c>
-      <c r="CL34" s="17" t="s">
+      <c r="CL34" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="CM34" s="16"/>
-      <c r="CN34" s="16"/>
-      <c r="CO34" s="16"/>
-      <c r="CP34" s="16"/>
-      <c r="CQ34" s="16"/>
-      <c r="CR34" s="16"/>
-      <c r="CS34" s="16"/>
-      <c r="CT34" s="15">
+      <c r="CM34" s="21"/>
+      <c r="CN34" s="21"/>
+      <c r="CO34" s="21"/>
+      <c r="CP34" s="21"/>
+      <c r="CQ34" s="21"/>
+      <c r="CR34" s="21"/>
+      <c r="CS34" s="21"/>
+      <c r="CT34" s="20">
         <v>2</v>
       </c>
-      <c r="CU34" s="17" t="s">
+      <c r="CU34" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="CV34" s="17" t="s">
+      <c r="CV34" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="CW34" s="17" t="s">
+      <c r="CW34" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="CX34" s="17" t="s">
+      <c r="CX34" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="CY34" s="27">
+      <c r="CY34" s="20">
         <v>28.6</v>
       </c>
-      <c r="CZ34" s="27">
+      <c r="CZ34" s="20">
         <v>28.6</v>
       </c>
-      <c r="DA34" s="15">
+      <c r="DA34" s="20">
         <v>1</v>
       </c>
-      <c r="DB34" s="17" t="s">
+      <c r="DB34" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="DC34" s="17" t="s">
+      <c r="DC34" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="DD34" s="17" t="s">
+      <c r="DD34" s="22" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="13"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15">
+    <row r="35" spans="2:108" ht="20" customHeight="1">
+      <c r="B35" s="18"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20">
         <v>95875321</v>
       </c>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="17" t="s">
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="N35" s="17" t="s">
+      <c r="N35" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="O35" s="16"/>
-      <c r="P35" s="15">
+      <c r="O35" s="21"/>
+      <c r="P35" s="20">
         <v>19690514</v>
       </c>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="16"/>
-      <c r="T35" s="16"/>
-      <c r="U35" s="16"/>
-      <c r="V35" s="16"/>
-      <c r="W35" s="16"/>
-      <c r="X35" s="16"/>
-      <c r="Y35" s="16"/>
-      <c r="Z35" s="16"/>
-      <c r="AA35" s="16"/>
-      <c r="AB35" s="16"/>
-      <c r="AC35" s="16"/>
-      <c r="AD35" s="16"/>
-      <c r="AE35" s="16"/>
-      <c r="AF35" s="16"/>
-      <c r="AG35" s="16"/>
-      <c r="AH35" s="16"/>
-      <c r="AI35" s="16"/>
-      <c r="AJ35" s="16"/>
-      <c r="AK35" s="16"/>
-      <c r="AL35" s="16"/>
-      <c r="AM35" s="16"/>
-      <c r="AN35" s="16"/>
-      <c r="AO35" s="16"/>
-      <c r="AP35" s="15">
+      <c r="Q35" s="21"/>
+      <c r="R35" s="21"/>
+      <c r="S35" s="21"/>
+      <c r="T35" s="21"/>
+      <c r="U35" s="21"/>
+      <c r="V35" s="21"/>
+      <c r="W35" s="21"/>
+      <c r="X35" s="21"/>
+      <c r="Y35" s="21"/>
+      <c r="Z35" s="21"/>
+      <c r="AA35" s="21"/>
+      <c r="AB35" s="21"/>
+      <c r="AC35" s="21"/>
+      <c r="AD35" s="21"/>
+      <c r="AE35" s="21"/>
+      <c r="AF35" s="21"/>
+      <c r="AG35" s="21"/>
+      <c r="AH35" s="21"/>
+      <c r="AI35" s="21"/>
+      <c r="AJ35" s="21"/>
+      <c r="AK35" s="21"/>
+      <c r="AL35" s="21"/>
+      <c r="AM35" s="21"/>
+      <c r="AN35" s="21"/>
+      <c r="AO35" s="21"/>
+      <c r="AP35" s="20">
         <v>19910411</v>
       </c>
-      <c r="AQ35" s="16"/>
-      <c r="AR35" s="17" t="s">
+      <c r="AQ35" s="21"/>
+      <c r="AR35" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="AS35" s="16"/>
-      <c r="AT35" s="16"/>
-      <c r="AU35" s="16"/>
-      <c r="AV35" s="16"/>
-      <c r="AW35" s="16"/>
-      <c r="AX35" s="17" t="s">
+      <c r="AS35" s="21"/>
+      <c r="AT35" s="21"/>
+      <c r="AU35" s="21"/>
+      <c r="AV35" s="21"/>
+      <c r="AW35" s="21"/>
+      <c r="AX35" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AY35" s="16"/>
-      <c r="AZ35" s="25">
+      <c r="AY35" s="21"/>
+      <c r="AZ35" s="26">
         <v>101001029000</v>
       </c>
-      <c r="BA35" s="16"/>
-      <c r="BB35" s="16"/>
-      <c r="BC35" s="16"/>
-      <c r="BD35" s="17" t="s">
+      <c r="BA35" s="21"/>
+      <c r="BB35" s="21"/>
+      <c r="BC35" s="21"/>
+      <c r="BD35" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="BE35" s="17" t="s">
+      <c r="BE35" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="BF35" s="17" t="s">
+      <c r="BF35" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="BG35" s="16"/>
-      <c r="BH35" s="16"/>
-      <c r="BI35" s="16"/>
-      <c r="BJ35" s="16"/>
-      <c r="BK35" s="16"/>
-      <c r="BL35" s="16"/>
-      <c r="BM35" s="16"/>
-      <c r="BN35" s="16"/>
-      <c r="BO35" s="16"/>
-      <c r="BP35" s="16"/>
-      <c r="BQ35" s="16"/>
-      <c r="BR35" s="16"/>
-      <c r="BS35" s="16"/>
-      <c r="BT35" s="16"/>
-      <c r="BU35" s="16"/>
-      <c r="BV35" s="16"/>
-      <c r="BW35" s="16"/>
-      <c r="BX35" s="16"/>
-      <c r="BY35" s="16"/>
-      <c r="BZ35" s="16"/>
-      <c r="CA35" s="16"/>
-      <c r="CB35" s="16"/>
-      <c r="CC35" s="16"/>
-      <c r="CD35" s="17" t="s">
+      <c r="BG35" s="21"/>
+      <c r="BH35" s="21"/>
+      <c r="BI35" s="21"/>
+      <c r="BJ35" s="21"/>
+      <c r="BK35" s="21"/>
+      <c r="BL35" s="21"/>
+      <c r="BM35" s="21"/>
+      <c r="BN35" s="21"/>
+      <c r="BO35" s="21"/>
+      <c r="BP35" s="21"/>
+      <c r="BQ35" s="21"/>
+      <c r="BR35" s="21"/>
+      <c r="BS35" s="21"/>
+      <c r="BT35" s="21"/>
+      <c r="BU35" s="21"/>
+      <c r="BV35" s="21"/>
+      <c r="BW35" s="21"/>
+      <c r="BX35" s="21"/>
+      <c r="BY35" s="21"/>
+      <c r="BZ35" s="21"/>
+      <c r="CA35" s="21"/>
+      <c r="CB35" s="21"/>
+      <c r="CC35" s="21"/>
+      <c r="CD35" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="CE35" s="17" t="s">
+      <c r="CE35" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="CF35" s="17" t="s">
+      <c r="CF35" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="CG35" s="16"/>
-      <c r="CH35" s="16"/>
-      <c r="CI35" s="16"/>
-      <c r="CJ35" s="17" t="s">
+      <c r="CG35" s="21"/>
+      <c r="CH35" s="21"/>
+      <c r="CI35" s="21"/>
+      <c r="CJ35" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="CK35" s="15">
+      <c r="CK35" s="20">
         <v>6</v>
       </c>
-      <c r="CL35" s="17" t="s">
+      <c r="CL35" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="CM35" s="16"/>
-      <c r="CN35" s="16"/>
-      <c r="CO35" s="16"/>
-      <c r="CP35" s="16"/>
-      <c r="CQ35" s="16"/>
-      <c r="CR35" s="16"/>
-      <c r="CS35" s="16"/>
-      <c r="CT35" s="16"/>
-      <c r="CU35" s="16"/>
-      <c r="CV35" s="16"/>
-      <c r="CW35" s="16"/>
-      <c r="CX35" s="16"/>
-      <c r="CY35" s="16"/>
-      <c r="CZ35" s="16"/>
-      <c r="DA35" s="16"/>
-      <c r="DB35" s="16"/>
-      <c r="DC35" s="16"/>
-      <c r="DD35" s="16"/>
+      <c r="CM35" s="21"/>
+      <c r="CN35" s="21"/>
+      <c r="CO35" s="21"/>
+      <c r="CP35" s="21"/>
+      <c r="CQ35" s="21"/>
+      <c r="CR35" s="21"/>
+      <c r="CS35" s="21"/>
+      <c r="CT35" s="20"/>
+      <c r="CU35" s="22"/>
+      <c r="CV35" s="22"/>
+      <c r="CW35" s="22"/>
+      <c r="CX35" s="22"/>
+      <c r="CY35" s="20"/>
+      <c r="CZ35" s="20"/>
+      <c r="DA35" s="20"/>
+      <c r="DB35" s="22"/>
+      <c r="DC35" s="22"/>
+      <c r="DD35" s="22"/>
     </row>
-    <row r="36" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20">
+    <row r="36" spans="2:108" ht="20" customHeight="1">
+      <c r="B36" s="13"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="15">
         <v>34499400</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="22" t="s">
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="N36" s="22" t="s">
+      <c r="N36" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="O36" s="21"/>
-      <c r="P36" s="20">
+      <c r="O36" s="16"/>
+      <c r="P36" s="15">
         <v>20060814</v>
       </c>
-      <c r="Q36" s="21"/>
-      <c r="R36" s="21"/>
-      <c r="S36" s="21"/>
-      <c r="T36" s="21"/>
-      <c r="U36" s="21"/>
-      <c r="V36" s="21"/>
-      <c r="W36" s="21"/>
-      <c r="X36" s="21"/>
-      <c r="Y36" s="21"/>
-      <c r="Z36" s="21"/>
-      <c r="AA36" s="21"/>
-      <c r="AB36" s="21"/>
-      <c r="AC36" s="21"/>
-      <c r="AD36" s="21"/>
-      <c r="AE36" s="21"/>
-      <c r="AF36" s="21"/>
-      <c r="AG36" s="21"/>
-      <c r="AH36" s="21"/>
-      <c r="AI36" s="21"/>
-      <c r="AJ36" s="21"/>
-      <c r="AK36" s="21"/>
-      <c r="AL36" s="21"/>
-      <c r="AM36" s="21"/>
-      <c r="AN36" s="21"/>
-      <c r="AO36" s="21"/>
-      <c r="AP36" s="20">
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16"/>
+      <c r="V36" s="16"/>
+      <c r="W36" s="16"/>
+      <c r="X36" s="16"/>
+      <c r="Y36" s="16"/>
+      <c r="Z36" s="16"/>
+      <c r="AA36" s="16"/>
+      <c r="AB36" s="16"/>
+      <c r="AC36" s="16"/>
+      <c r="AD36" s="16"/>
+      <c r="AE36" s="16"/>
+      <c r="AF36" s="16"/>
+      <c r="AG36" s="16"/>
+      <c r="AH36" s="16"/>
+      <c r="AI36" s="16"/>
+      <c r="AJ36" s="16"/>
+      <c r="AK36" s="16"/>
+      <c r="AL36" s="16"/>
+      <c r="AM36" s="16"/>
+      <c r="AN36" s="16"/>
+      <c r="AO36" s="16"/>
+      <c r="AP36" s="15">
         <v>20080410</v>
       </c>
-      <c r="AQ36" s="21"/>
-      <c r="AR36" s="22" t="s">
+      <c r="AQ36" s="16"/>
+      <c r="AR36" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AS36" s="21"/>
-      <c r="AT36" s="21"/>
-      <c r="AU36" s="21"/>
-      <c r="AV36" s="21"/>
-      <c r="AW36" s="21"/>
-      <c r="AX36" s="22" t="s">
+      <c r="AS36" s="16"/>
+      <c r="AT36" s="16"/>
+      <c r="AU36" s="16"/>
+      <c r="AV36" s="16"/>
+      <c r="AW36" s="16"/>
+      <c r="AX36" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="AY36" s="21"/>
-      <c r="AZ36" s="26">
+      <c r="AY36" s="16"/>
+      <c r="AZ36" s="25">
         <v>101001030000</v>
       </c>
-      <c r="BA36" s="21"/>
-      <c r="BB36" s="21"/>
-      <c r="BC36" s="21"/>
-      <c r="BD36" s="22" t="s">
+      <c r="BA36" s="16"/>
+      <c r="BB36" s="16"/>
+      <c r="BC36" s="16"/>
+      <c r="BD36" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="BE36" s="22" t="s">
+      <c r="BE36" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="BF36" s="21"/>
-      <c r="BG36" s="21"/>
-      <c r="BH36" s="21"/>
-      <c r="BI36" s="21"/>
-      <c r="BJ36" s="21"/>
-      <c r="BK36" s="21"/>
-      <c r="BL36" s="21"/>
-      <c r="BM36" s="21"/>
-      <c r="BN36" s="21"/>
-      <c r="BO36" s="21"/>
-      <c r="BP36" s="21"/>
-      <c r="BQ36" s="21"/>
-      <c r="BR36" s="21"/>
-      <c r="BS36" s="21"/>
-      <c r="BT36" s="21"/>
-      <c r="BU36" s="21"/>
-      <c r="BV36" s="21"/>
-      <c r="BW36" s="21"/>
-      <c r="BX36" s="21"/>
-      <c r="BY36" s="21"/>
-      <c r="BZ36" s="21"/>
-      <c r="CA36" s="21"/>
-      <c r="CB36" s="21"/>
-      <c r="CC36" s="21"/>
-      <c r="CD36" s="22" t="s">
+      <c r="BF36" s="16"/>
+      <c r="BG36" s="16"/>
+      <c r="BH36" s="16"/>
+      <c r="BI36" s="16"/>
+      <c r="BJ36" s="16"/>
+      <c r="BK36" s="16"/>
+      <c r="BL36" s="16"/>
+      <c r="BM36" s="16"/>
+      <c r="BN36" s="16"/>
+      <c r="BO36" s="16"/>
+      <c r="BP36" s="16"/>
+      <c r="BQ36" s="16"/>
+      <c r="BR36" s="16"/>
+      <c r="BS36" s="16"/>
+      <c r="BT36" s="16"/>
+      <c r="BU36" s="16"/>
+      <c r="BV36" s="16"/>
+      <c r="BW36" s="16"/>
+      <c r="BX36" s="16"/>
+      <c r="BY36" s="16"/>
+      <c r="BZ36" s="16"/>
+      <c r="CA36" s="16"/>
+      <c r="CB36" s="16"/>
+      <c r="CC36" s="16"/>
+      <c r="CD36" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="CE36" s="21"/>
-      <c r="CF36" s="22" t="s">
+      <c r="CE36" s="16"/>
+      <c r="CF36" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="CG36" s="21"/>
-      <c r="CH36" s="21"/>
-      <c r="CI36" s="21"/>
-      <c r="CJ36" s="22" t="s">
+      <c r="CG36" s="16"/>
+      <c r="CH36" s="16"/>
+      <c r="CI36" s="16"/>
+      <c r="CJ36" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="CK36" s="20">
+      <c r="CK36" s="15">
         <v>10</v>
       </c>
-      <c r="CL36" s="22" t="s">
+      <c r="CL36" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="CM36" s="21"/>
-      <c r="CN36" s="21"/>
-      <c r="CO36" s="21"/>
-      <c r="CP36" s="21"/>
-      <c r="CQ36" s="21"/>
-      <c r="CR36" s="21"/>
-      <c r="CS36" s="21"/>
-      <c r="CT36" s="20">
+      <c r="CM36" s="16"/>
+      <c r="CN36" s="16"/>
+      <c r="CO36" s="16"/>
+      <c r="CP36" s="16"/>
+      <c r="CQ36" s="16"/>
+      <c r="CR36" s="16"/>
+      <c r="CS36" s="16"/>
+      <c r="CT36" s="15">
         <v>1</v>
       </c>
-      <c r="CU36" s="22" t="s">
+      <c r="CU36" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="CV36" s="22" t="s">
+      <c r="CV36" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="CW36" s="22" t="s">
+      <c r="CW36" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="CX36" s="22" t="s">
+      <c r="CX36" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="CY36" s="20">
+      <c r="CY36" s="15">
         <v>11.6</v>
       </c>
-      <c r="CZ36" s="20">
+      <c r="CZ36" s="15">
         <v>11.6</v>
       </c>
-      <c r="DA36" s="20">
+      <c r="DA36" s="15">
         <v>1</v>
       </c>
-      <c r="DB36" s="22" t="s">
+      <c r="DB36" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="DC36" s="22" t="s">
+      <c r="DC36" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="DD36" s="22" t="s">
+      <c r="DD36" s="17" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="37" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="13"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="15">
+    <row r="37" spans="2:108" ht="20" customHeight="1">
+      <c r="B37" s="18"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="20">
         <v>43322421</v>
       </c>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="17" t="s">
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="N37" s="17" t="s">
+      <c r="N37" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="O37" s="16"/>
-      <c r="P37" s="15">
+      <c r="O37" s="21"/>
+      <c r="P37" s="20">
         <v>19831119</v>
       </c>
-      <c r="Q37" s="16"/>
-      <c r="R37" s="16"/>
-      <c r="S37" s="16"/>
-      <c r="T37" s="16"/>
-      <c r="U37" s="16"/>
-      <c r="V37" s="16"/>
-      <c r="W37" s="16"/>
-      <c r="X37" s="16"/>
-      <c r="Y37" s="16"/>
-      <c r="Z37" s="16"/>
-      <c r="AA37" s="16"/>
-      <c r="AB37" s="16"/>
-      <c r="AC37" s="16"/>
-      <c r="AD37" s="16"/>
-      <c r="AE37" s="16"/>
-      <c r="AF37" s="16"/>
-      <c r="AG37" s="16"/>
-      <c r="AH37" s="16"/>
-      <c r="AI37" s="16"/>
-      <c r="AJ37" s="16"/>
-      <c r="AK37" s="16"/>
-      <c r="AL37" s="16"/>
-      <c r="AM37" s="16"/>
-      <c r="AN37" s="16"/>
-      <c r="AO37" s="16"/>
-      <c r="AP37" s="15">
+      <c r="Q37" s="21"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="21"/>
+      <c r="U37" s="21"/>
+      <c r="V37" s="21"/>
+      <c r="W37" s="21"/>
+      <c r="X37" s="21"/>
+      <c r="Y37" s="21"/>
+      <c r="Z37" s="21"/>
+      <c r="AA37" s="21"/>
+      <c r="AB37" s="21"/>
+      <c r="AC37" s="21"/>
+      <c r="AD37" s="21"/>
+      <c r="AE37" s="21"/>
+      <c r="AF37" s="21"/>
+      <c r="AG37" s="21"/>
+      <c r="AH37" s="21"/>
+      <c r="AI37" s="21"/>
+      <c r="AJ37" s="21"/>
+      <c r="AK37" s="21"/>
+      <c r="AL37" s="21"/>
+      <c r="AM37" s="21"/>
+      <c r="AN37" s="21"/>
+      <c r="AO37" s="21"/>
+      <c r="AP37" s="20">
         <v>20150214</v>
       </c>
-      <c r="AQ37" s="16"/>
-      <c r="AR37" s="17" t="s">
+      <c r="AQ37" s="21"/>
+      <c r="AR37" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="AS37" s="16"/>
-      <c r="AT37" s="16"/>
-      <c r="AU37" s="16"/>
-      <c r="AV37" s="16"/>
-      <c r="AW37" s="16"/>
-      <c r="AX37" s="17" t="s">
+      <c r="AS37" s="21"/>
+      <c r="AT37" s="21"/>
+      <c r="AU37" s="21"/>
+      <c r="AV37" s="21"/>
+      <c r="AW37" s="21"/>
+      <c r="AX37" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AY37" s="16"/>
-      <c r="AZ37" s="25">
+      <c r="AY37" s="21"/>
+      <c r="AZ37" s="26">
         <v>101001031000</v>
       </c>
-      <c r="BA37" s="16"/>
-      <c r="BB37" s="16"/>
-      <c r="BC37" s="16"/>
-      <c r="BD37" s="17" t="s">
+      <c r="BA37" s="21"/>
+      <c r="BB37" s="21"/>
+      <c r="BC37" s="21"/>
+      <c r="BD37" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="BE37" s="17" t="s">
+      <c r="BE37" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="BF37" s="16"/>
-      <c r="BG37" s="16"/>
-      <c r="BH37" s="16"/>
-      <c r="BI37" s="16"/>
-      <c r="BJ37" s="16"/>
-      <c r="BK37" s="16"/>
-      <c r="BL37" s="16"/>
-      <c r="BM37" s="16"/>
-      <c r="BN37" s="16"/>
-      <c r="BO37" s="16"/>
-      <c r="BP37" s="16"/>
-      <c r="BQ37" s="16"/>
-      <c r="BR37" s="16"/>
-      <c r="BS37" s="16"/>
-      <c r="BT37" s="16"/>
-      <c r="BU37" s="16"/>
-      <c r="BV37" s="16"/>
-      <c r="BW37" s="16"/>
-      <c r="BX37" s="16"/>
-      <c r="BY37" s="16"/>
-      <c r="BZ37" s="16"/>
-      <c r="CA37" s="16"/>
-      <c r="CB37" s="16"/>
-      <c r="CC37" s="16"/>
-      <c r="CD37" s="17" t="s">
+      <c r="BF37" s="21"/>
+      <c r="BG37" s="21"/>
+      <c r="BH37" s="21"/>
+      <c r="BI37" s="21"/>
+      <c r="BJ37" s="21"/>
+      <c r="BK37" s="21"/>
+      <c r="BL37" s="21"/>
+      <c r="BM37" s="21"/>
+      <c r="BN37" s="21"/>
+      <c r="BO37" s="21"/>
+      <c r="BP37" s="21"/>
+      <c r="BQ37" s="21"/>
+      <c r="BR37" s="21"/>
+      <c r="BS37" s="21"/>
+      <c r="BT37" s="21"/>
+      <c r="BU37" s="21"/>
+      <c r="BV37" s="21"/>
+      <c r="BW37" s="21"/>
+      <c r="BX37" s="21"/>
+      <c r="BY37" s="21"/>
+      <c r="BZ37" s="21"/>
+      <c r="CA37" s="21"/>
+      <c r="CB37" s="21"/>
+      <c r="CC37" s="21"/>
+      <c r="CD37" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="CE37" s="16"/>
-      <c r="CF37" s="17" t="s">
+      <c r="CE37" s="21"/>
+      <c r="CF37" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="CG37" s="16"/>
-      <c r="CH37" s="16"/>
-      <c r="CI37" s="16"/>
-      <c r="CJ37" s="17" t="s">
+      <c r="CG37" s="21"/>
+      <c r="CH37" s="21"/>
+      <c r="CI37" s="21"/>
+      <c r="CJ37" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="CK37" s="15">
+      <c r="CK37" s="21">
         <v>5</v>
       </c>
-      <c r="CL37" s="17" t="s">
+      <c r="CL37" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="CM37" s="16"/>
-      <c r="CN37" s="16"/>
-      <c r="CO37" s="16"/>
-      <c r="CP37" s="16"/>
-      <c r="CQ37" s="16"/>
-      <c r="CR37" s="16"/>
-      <c r="CS37" s="16"/>
-      <c r="CT37" s="15">
+      <c r="CM37" s="21"/>
+      <c r="CN37" s="21"/>
+      <c r="CO37" s="21"/>
+      <c r="CP37" s="21"/>
+      <c r="CQ37" s="21"/>
+      <c r="CR37" s="21"/>
+      <c r="CS37" s="21"/>
+      <c r="CT37" s="21">
         <v>1</v>
       </c>
-      <c r="CU37" s="17" t="s">
+      <c r="CU37" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="CV37" s="17" t="s">
+      <c r="CV37" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="CW37" s="17" t="s">
+      <c r="CW37" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="CX37" s="17" t="s">
+      <c r="CX37" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="CY37" s="15">
+      <c r="CY37" s="21">
         <v>4.7</v>
       </c>
-      <c r="CZ37" s="15">
+      <c r="CZ37" s="21">
         <v>4.7</v>
       </c>
-      <c r="DA37" s="15">
+      <c r="DA37" s="21">
         <v>1</v>
       </c>
-      <c r="DB37" s="17" t="s">
+      <c r="DB37" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="DC37" s="17" t="s">
+      <c r="DC37" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="DD37" s="17" t="s">
+      <c r="DD37" s="21" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20">
+    <row r="38" spans="2:108" ht="20" customHeight="1">
+      <c r="B38" s="13"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="15">
         <v>66678381</v>
       </c>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="22" t="s">
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="N38" s="22" t="s">
+      <c r="N38" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="O38" s="21"/>
-      <c r="P38" s="20">
+      <c r="O38" s="16"/>
+      <c r="P38" s="15">
         <v>19990519</v>
       </c>
-      <c r="Q38" s="21"/>
-      <c r="R38" s="21"/>
-      <c r="S38" s="21"/>
-      <c r="T38" s="21"/>
-      <c r="U38" s="21"/>
-      <c r="V38" s="21"/>
-      <c r="W38" s="21"/>
-      <c r="X38" s="21"/>
-      <c r="Y38" s="21"/>
-      <c r="Z38" s="21"/>
-      <c r="AA38" s="21"/>
-      <c r="AB38" s="21"/>
-      <c r="AC38" s="21"/>
-      <c r="AD38" s="21"/>
-      <c r="AE38" s="21"/>
-      <c r="AF38" s="21"/>
-      <c r="AG38" s="21"/>
-      <c r="AH38" s="21"/>
-      <c r="AI38" s="21"/>
-      <c r="AJ38" s="21"/>
-      <c r="AK38" s="21"/>
-      <c r="AL38" s="21"/>
-      <c r="AM38" s="21"/>
-      <c r="AN38" s="21"/>
-      <c r="AO38" s="21"/>
-      <c r="AP38" s="20">
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
+      <c r="V38" s="16"/>
+      <c r="W38" s="16"/>
+      <c r="X38" s="16"/>
+      <c r="Y38" s="16"/>
+      <c r="Z38" s="16"/>
+      <c r="AA38" s="16"/>
+      <c r="AB38" s="16"/>
+      <c r="AC38" s="16"/>
+      <c r="AD38" s="16"/>
+      <c r="AE38" s="16"/>
+      <c r="AF38" s="16"/>
+      <c r="AG38" s="16"/>
+      <c r="AH38" s="16"/>
+      <c r="AI38" s="16"/>
+      <c r="AJ38" s="16"/>
+      <c r="AK38" s="16"/>
+      <c r="AL38" s="16"/>
+      <c r="AM38" s="16"/>
+      <c r="AN38" s="16"/>
+      <c r="AO38" s="16"/>
+      <c r="AP38" s="15">
         <v>20030410</v>
       </c>
-      <c r="AQ38" s="21"/>
-      <c r="AR38" s="22" t="s">
+      <c r="AQ38" s="16"/>
+      <c r="AR38" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="AS38" s="21"/>
-      <c r="AT38" s="21"/>
-      <c r="AU38" s="21"/>
-      <c r="AV38" s="21"/>
-      <c r="AW38" s="21"/>
-      <c r="AX38" s="22" t="s">
+      <c r="AS38" s="16"/>
+      <c r="AT38" s="16"/>
+      <c r="AU38" s="16"/>
+      <c r="AV38" s="16"/>
+      <c r="AW38" s="16"/>
+      <c r="AX38" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="AY38" s="21"/>
-      <c r="AZ38" s="26">
+      <c r="AY38" s="16"/>
+      <c r="AZ38" s="25">
         <v>101001031000</v>
       </c>
-      <c r="BA38" s="21"/>
-      <c r="BB38" s="21"/>
-      <c r="BC38" s="21"/>
-      <c r="BD38" s="22" t="s">
+      <c r="BA38" s="16"/>
+      <c r="BB38" s="16"/>
+      <c r="BC38" s="16"/>
+      <c r="BD38" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="BE38" s="22" t="s">
+      <c r="BE38" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="BF38" s="21"/>
-      <c r="BG38" s="21"/>
-      <c r="BH38" s="21"/>
-      <c r="BI38" s="21"/>
-      <c r="BJ38" s="21"/>
-      <c r="BK38" s="21"/>
-      <c r="BL38" s="21"/>
-      <c r="BM38" s="21"/>
-      <c r="BN38" s="21"/>
-      <c r="BO38" s="21"/>
-      <c r="BP38" s="21"/>
-      <c r="BQ38" s="21"/>
-      <c r="BR38" s="21"/>
-      <c r="BS38" s="21"/>
-      <c r="BT38" s="21"/>
-      <c r="BU38" s="21"/>
-      <c r="BV38" s="21"/>
-      <c r="BW38" s="21"/>
-      <c r="BX38" s="21"/>
-      <c r="BY38" s="21"/>
-      <c r="BZ38" s="21"/>
-      <c r="CA38" s="21"/>
-      <c r="CB38" s="21"/>
-      <c r="CC38" s="21"/>
-      <c r="CD38" s="21"/>
-      <c r="CE38" s="21"/>
-      <c r="CF38" s="21"/>
-      <c r="CG38" s="21"/>
-      <c r="CH38" s="21"/>
-      <c r="CI38" s="21"/>
-      <c r="CJ38" s="21"/>
-      <c r="CK38" s="21"/>
-      <c r="CL38" s="21"/>
-      <c r="CM38" s="21"/>
-      <c r="CN38" s="21"/>
-      <c r="CO38" s="21"/>
-      <c r="CP38" s="21"/>
-      <c r="CQ38" s="21"/>
-      <c r="CR38" s="21"/>
-      <c r="CS38" s="21"/>
-      <c r="CT38" s="21"/>
-      <c r="CU38" s="21"/>
-      <c r="CV38" s="21"/>
-      <c r="CW38" s="21"/>
-      <c r="CX38" s="21"/>
-      <c r="CY38" s="21"/>
-      <c r="CZ38" s="21"/>
-      <c r="DA38" s="21"/>
-      <c r="DB38" s="21"/>
-      <c r="DC38" s="21"/>
-      <c r="DD38" s="21"/>
+      <c r="BF38" s="16"/>
+      <c r="BG38" s="16"/>
+      <c r="BH38" s="16"/>
+      <c r="BI38" s="16"/>
+      <c r="BJ38" s="16"/>
+      <c r="BK38" s="16"/>
+      <c r="BL38" s="16"/>
+      <c r="BM38" s="16"/>
+      <c r="BN38" s="16"/>
+      <c r="BO38" s="16"/>
+      <c r="BP38" s="16"/>
+      <c r="BQ38" s="16"/>
+      <c r="BR38" s="16"/>
+      <c r="BS38" s="16"/>
+      <c r="BT38" s="16"/>
+      <c r="BU38" s="16"/>
+      <c r="BV38" s="16"/>
+      <c r="BW38" s="16"/>
+      <c r="BX38" s="16"/>
+      <c r="BY38" s="16"/>
+      <c r="BZ38" s="16"/>
+      <c r="CA38" s="16"/>
+      <c r="CB38" s="16"/>
+      <c r="CC38" s="16"/>
+      <c r="CD38" s="17"/>
+      <c r="CE38" s="16"/>
+      <c r="CF38" s="17"/>
+      <c r="CG38" s="16"/>
+      <c r="CH38" s="16"/>
+      <c r="CI38" s="16"/>
+      <c r="CJ38" s="16"/>
+      <c r="CK38" s="16"/>
+      <c r="CL38" s="16"/>
+      <c r="CM38" s="16"/>
+      <c r="CN38" s="16"/>
+      <c r="CO38" s="16"/>
+      <c r="CP38" s="16"/>
+      <c r="CQ38" s="16"/>
+      <c r="CR38" s="16"/>
+      <c r="CS38" s="16"/>
+      <c r="CT38" s="16"/>
+      <c r="CU38" s="16"/>
+      <c r="CV38" s="16"/>
+      <c r="CW38" s="16"/>
+      <c r="CX38" s="16"/>
+      <c r="CY38" s="16"/>
+      <c r="CZ38" s="16"/>
+      <c r="DA38" s="16"/>
+      <c r="DB38" s="16"/>
+      <c r="DC38" s="16"/>
+      <c r="DD38" s="16"/>
     </row>
-    <row r="39" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" s="18"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="20">
+    <row r="39" spans="2:108" ht="20" customHeight="1">
+      <c r="B39" s="13"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="15">
         <v>66678381</v>
       </c>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="22" t="s">
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="N39" s="22" t="s">
+      <c r="N39" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="O39" s="21"/>
-      <c r="P39" s="20">
+      <c r="O39" s="16"/>
+      <c r="P39" s="15">
         <v>19990519</v>
       </c>
-      <c r="Q39" s="21"/>
-      <c r="R39" s="21"/>
-      <c r="S39" s="21"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="21"/>
-      <c r="V39" s="21"/>
-      <c r="W39" s="21"/>
-      <c r="X39" s="21"/>
-      <c r="Y39" s="21"/>
-      <c r="Z39" s="21"/>
-      <c r="AA39" s="21"/>
-      <c r="AB39" s="21"/>
-      <c r="AC39" s="21"/>
-      <c r="AD39" s="21"/>
-      <c r="AE39" s="21"/>
-      <c r="AF39" s="21"/>
-      <c r="AG39" s="21"/>
-      <c r="AH39" s="21"/>
-      <c r="AI39" s="21"/>
-      <c r="AJ39" s="21"/>
-      <c r="AK39" s="21"/>
-      <c r="AL39" s="21"/>
-      <c r="AM39" s="21"/>
-      <c r="AN39" s="21"/>
-      <c r="AO39" s="21"/>
-      <c r="AP39" s="20">
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
+      <c r="V39" s="16"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="16"/>
+      <c r="Y39" s="16"/>
+      <c r="Z39" s="16"/>
+      <c r="AA39" s="16"/>
+      <c r="AB39" s="16"/>
+      <c r="AC39" s="16"/>
+      <c r="AD39" s="16"/>
+      <c r="AE39" s="16"/>
+      <c r="AF39" s="16"/>
+      <c r="AG39" s="16"/>
+      <c r="AH39" s="16"/>
+      <c r="AI39" s="16"/>
+      <c r="AJ39" s="16"/>
+      <c r="AK39" s="16"/>
+      <c r="AL39" s="16"/>
+      <c r="AM39" s="16"/>
+      <c r="AN39" s="16"/>
+      <c r="AO39" s="16"/>
+      <c r="AP39" s="15">
         <v>20150214</v>
       </c>
-      <c r="AQ39" s="21"/>
-      <c r="AR39" s="22" t="s">
+      <c r="AQ39" s="16"/>
+      <c r="AR39" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AS39" s="21"/>
-      <c r="AT39" s="21"/>
-      <c r="AU39" s="21"/>
-      <c r="AV39" s="21"/>
-      <c r="AW39" s="21"/>
-      <c r="AX39" s="22" t="s">
+      <c r="AS39" s="16"/>
+      <c r="AT39" s="16"/>
+      <c r="AU39" s="16"/>
+      <c r="AV39" s="16"/>
+      <c r="AW39" s="16"/>
+      <c r="AX39" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="AY39" s="21"/>
-      <c r="AZ39" s="26">
+      <c r="AY39" s="16"/>
+      <c r="AZ39" s="25">
         <v>101001034000</v>
       </c>
-      <c r="BA39" s="21"/>
-      <c r="BB39" s="21"/>
-      <c r="BC39" s="21"/>
-      <c r="BD39" s="22" t="s">
+      <c r="BA39" s="16"/>
+      <c r="BB39" s="16"/>
+      <c r="BC39" s="16"/>
+      <c r="BD39" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="BE39" s="22" t="s">
+      <c r="BE39" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="BF39" s="21"/>
-      <c r="BG39" s="21"/>
-      <c r="BH39" s="21"/>
-      <c r="BI39" s="21"/>
-      <c r="BJ39" s="21"/>
-      <c r="BK39" s="21"/>
-      <c r="BL39" s="21"/>
-      <c r="BM39" s="21"/>
-      <c r="BN39" s="21"/>
-      <c r="BO39" s="21"/>
-      <c r="BP39" s="21"/>
-      <c r="BQ39" s="21"/>
-      <c r="BR39" s="21"/>
-      <c r="BS39" s="21"/>
-      <c r="BT39" s="21"/>
-      <c r="BU39" s="21"/>
-      <c r="BV39" s="21"/>
-      <c r="BW39" s="21"/>
-      <c r="BX39" s="21"/>
-      <c r="BY39" s="21"/>
-      <c r="BZ39" s="21"/>
-      <c r="CA39" s="21"/>
-      <c r="CB39" s="21"/>
-      <c r="CC39" s="21"/>
-      <c r="CD39" s="22" t="s">
+      <c r="BF39" s="16"/>
+      <c r="BG39" s="16"/>
+      <c r="BH39" s="16"/>
+      <c r="BI39" s="16"/>
+      <c r="BJ39" s="16"/>
+      <c r="BK39" s="16"/>
+      <c r="BL39" s="16"/>
+      <c r="BM39" s="16"/>
+      <c r="BN39" s="16"/>
+      <c r="BO39" s="16"/>
+      <c r="BP39" s="16"/>
+      <c r="BQ39" s="16"/>
+      <c r="BR39" s="16"/>
+      <c r="BS39" s="16"/>
+      <c r="BT39" s="16"/>
+      <c r="BU39" s="16"/>
+      <c r="BV39" s="16"/>
+      <c r="BW39" s="16"/>
+      <c r="BX39" s="16"/>
+      <c r="BY39" s="16"/>
+      <c r="BZ39" s="16"/>
+      <c r="CA39" s="16"/>
+      <c r="CB39" s="16"/>
+      <c r="CC39" s="16"/>
+      <c r="CD39" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="CE39" s="22" t="s">
+      <c r="CE39" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="CF39" s="22" t="s">
+      <c r="CF39" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="CG39" s="21"/>
-      <c r="CH39" s="21"/>
-      <c r="CI39" s="21"/>
-      <c r="CJ39" s="22" t="s">
+      <c r="CG39" s="16"/>
+      <c r="CH39" s="16"/>
+      <c r="CI39" s="16"/>
+      <c r="CJ39" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="CK39" s="20">
+      <c r="CK39" s="16">
         <v>30</v>
       </c>
-      <c r="CL39" s="22" t="s">
+      <c r="CL39" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="CM39" s="21"/>
-      <c r="CN39" s="21"/>
-      <c r="CO39" s="21"/>
-      <c r="CP39" s="21"/>
-      <c r="CQ39" s="21"/>
-      <c r="CR39" s="21"/>
-      <c r="CS39" s="21"/>
-      <c r="CT39" s="20">
+      <c r="CM39" s="16"/>
+      <c r="CN39" s="16"/>
+      <c r="CO39" s="16"/>
+      <c r="CP39" s="16"/>
+      <c r="CQ39" s="16"/>
+      <c r="CR39" s="16"/>
+      <c r="CS39" s="16"/>
+      <c r="CT39" s="16">
         <v>1</v>
       </c>
-      <c r="CU39" s="22" t="s">
+      <c r="CU39" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="CV39" s="22" t="s">
+      <c r="CV39" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="CW39" s="22" t="s">
+      <c r="CW39" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="CX39" s="22" t="s">
+      <c r="CX39" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="CY39" s="20">
+      <c r="CY39" s="16">
         <v>4.7</v>
       </c>
-      <c r="CZ39" s="20">
+      <c r="CZ39" s="16">
         <v>4.7</v>
       </c>
-      <c r="DA39" s="20">
+      <c r="DA39" s="16">
         <v>0</v>
       </c>
-      <c r="DB39" s="22" t="s">
+      <c r="DB39" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="DC39" s="22" t="s">
+      <c r="DC39" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="DD39" s="22" t="s">
+      <c r="DD39" s="16" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B40" s="13"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="15">
+    <row r="40" spans="2:108" ht="20" customHeight="1">
+      <c r="B40" s="18"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="20">
         <v>34174567</v>
       </c>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="16"/>
-      <c r="K40" s="16"/>
-      <c r="L40" s="16"/>
-      <c r="M40" s="17" t="s">
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="N40" s="17" t="s">
+      <c r="N40" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="O40" s="16"/>
-      <c r="P40" s="15">
+      <c r="O40" s="21"/>
+      <c r="P40" s="20">
         <v>19240811</v>
       </c>
-      <c r="Q40" s="16"/>
-      <c r="R40" s="16"/>
-      <c r="S40" s="16"/>
-      <c r="T40" s="16"/>
-      <c r="U40" s="16"/>
-      <c r="V40" s="16"/>
-      <c r="W40" s="16"/>
-      <c r="X40" s="16"/>
-      <c r="Y40" s="16"/>
-      <c r="Z40" s="16"/>
-      <c r="AA40" s="16"/>
-      <c r="AB40" s="16"/>
-      <c r="AC40" s="16"/>
-      <c r="AD40" s="16"/>
-      <c r="AE40" s="16"/>
-      <c r="AF40" s="16"/>
-      <c r="AG40" s="16"/>
-      <c r="AH40" s="16"/>
-      <c r="AI40" s="16"/>
-      <c r="AJ40" s="16"/>
-      <c r="AK40" s="16"/>
-      <c r="AL40" s="16"/>
-      <c r="AM40" s="16"/>
-      <c r="AN40" s="16"/>
-      <c r="AO40" s="16"/>
-      <c r="AP40" s="15">
+      <c r="Q40" s="21"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="21"/>
+      <c r="U40" s="21"/>
+      <c r="V40" s="21"/>
+      <c r="W40" s="21"/>
+      <c r="X40" s="21"/>
+      <c r="Y40" s="21"/>
+      <c r="Z40" s="21"/>
+      <c r="AA40" s="21"/>
+      <c r="AB40" s="21"/>
+      <c r="AC40" s="21"/>
+      <c r="AD40" s="21"/>
+      <c r="AE40" s="21"/>
+      <c r="AF40" s="21"/>
+      <c r="AG40" s="21"/>
+      <c r="AH40" s="21"/>
+      <c r="AI40" s="21"/>
+      <c r="AJ40" s="21"/>
+      <c r="AK40" s="21"/>
+      <c r="AL40" s="21"/>
+      <c r="AM40" s="21"/>
+      <c r="AN40" s="21"/>
+      <c r="AO40" s="21"/>
+      <c r="AP40" s="20">
         <v>20050214</v>
       </c>
-      <c r="AQ40" s="16"/>
-      <c r="AR40" s="17" t="s">
+      <c r="AQ40" s="21"/>
+      <c r="AR40" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="AS40" s="16"/>
-      <c r="AT40" s="16"/>
-      <c r="AU40" s="16"/>
-      <c r="AV40" s="16"/>
-      <c r="AW40" s="16"/>
-      <c r="AX40" s="17" t="s">
+      <c r="AS40" s="21"/>
+      <c r="AT40" s="21"/>
+      <c r="AU40" s="21"/>
+      <c r="AV40" s="21"/>
+      <c r="AW40" s="21"/>
+      <c r="AX40" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AY40" s="16"/>
-      <c r="AZ40" s="25">
+      <c r="AY40" s="21"/>
+      <c r="AZ40" s="26">
         <v>101001034000</v>
       </c>
-      <c r="BA40" s="16"/>
-      <c r="BB40" s="16"/>
-      <c r="BC40" s="16"/>
-      <c r="BD40" s="17" t="s">
+      <c r="BA40" s="21"/>
+      <c r="BB40" s="21"/>
+      <c r="BC40" s="21"/>
+      <c r="BD40" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="BE40" s="17" t="s">
+      <c r="BE40" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="BF40" s="16"/>
-      <c r="BG40" s="16"/>
-      <c r="BH40" s="16"/>
-      <c r="BI40" s="16"/>
-      <c r="BJ40" s="16"/>
-      <c r="BK40" s="16"/>
-      <c r="BL40" s="16"/>
-      <c r="BM40" s="16"/>
-      <c r="BN40" s="16"/>
-      <c r="BO40" s="16"/>
-      <c r="BP40" s="16"/>
-      <c r="BQ40" s="16"/>
-      <c r="BR40" s="16"/>
-      <c r="BS40" s="16"/>
-      <c r="BT40" s="16"/>
-      <c r="BU40" s="16"/>
-      <c r="BV40" s="16"/>
-      <c r="BW40" s="16"/>
-      <c r="BX40" s="16"/>
-      <c r="BY40" s="16"/>
-      <c r="BZ40" s="16"/>
-      <c r="CA40" s="16"/>
-      <c r="CB40" s="16"/>
-      <c r="CC40" s="16"/>
-      <c r="CD40" s="17" t="s">
+      <c r="BF40" s="21"/>
+      <c r="BG40" s="21"/>
+      <c r="BH40" s="21"/>
+      <c r="BI40" s="21"/>
+      <c r="BJ40" s="21"/>
+      <c r="BK40" s="21"/>
+      <c r="BL40" s="21"/>
+      <c r="BM40" s="21"/>
+      <c r="BN40" s="21"/>
+      <c r="BO40" s="21"/>
+      <c r="BP40" s="21"/>
+      <c r="BQ40" s="21"/>
+      <c r="BR40" s="21"/>
+      <c r="BS40" s="21"/>
+      <c r="BT40" s="21"/>
+      <c r="BU40" s="21"/>
+      <c r="BV40" s="21"/>
+      <c r="BW40" s="21"/>
+      <c r="BX40" s="21"/>
+      <c r="BY40" s="21"/>
+      <c r="BZ40" s="21"/>
+      <c r="CA40" s="21"/>
+      <c r="CB40" s="21"/>
+      <c r="CC40" s="21"/>
+      <c r="CD40" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="CE40" s="16"/>
-      <c r="CF40" s="17" t="s">
+      <c r="CE40" s="21"/>
+      <c r="CF40" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="CG40" s="16"/>
-      <c r="CH40" s="16"/>
-      <c r="CI40" s="16"/>
-      <c r="CJ40" s="16"/>
-      <c r="CK40" s="16"/>
-      <c r="CL40" s="16"/>
-      <c r="CM40" s="16"/>
-      <c r="CN40" s="16"/>
-      <c r="CO40" s="16"/>
-      <c r="CP40" s="16"/>
-      <c r="CQ40" s="16"/>
-      <c r="CR40" s="16"/>
-      <c r="CS40" s="16"/>
-      <c r="CT40" s="16"/>
-      <c r="CU40" s="16"/>
-      <c r="CV40" s="16"/>
-      <c r="CW40" s="16"/>
-      <c r="CX40" s="16"/>
-      <c r="CY40" s="16"/>
-      <c r="CZ40" s="16"/>
-      <c r="DA40" s="16"/>
-      <c r="DB40" s="16"/>
-      <c r="DC40" s="16"/>
-      <c r="DD40" s="16"/>
+      <c r="CG40" s="21"/>
+      <c r="CH40" s="21"/>
+      <c r="CI40" s="21"/>
+      <c r="CJ40" s="22"/>
+      <c r="CK40" s="20"/>
+      <c r="CL40" s="22"/>
+      <c r="CM40" s="21"/>
+      <c r="CN40" s="21"/>
+      <c r="CO40" s="21"/>
+      <c r="CP40" s="21"/>
+      <c r="CQ40" s="21"/>
+      <c r="CR40" s="21"/>
+      <c r="CS40" s="21"/>
+      <c r="CT40" s="21"/>
+      <c r="CU40" s="21"/>
+      <c r="CV40" s="21"/>
+      <c r="CW40" s="21"/>
+      <c r="CX40" s="21"/>
+      <c r="CY40" s="21"/>
+      <c r="CZ40" s="21"/>
+      <c r="DA40" s="21"/>
+      <c r="DB40" s="21"/>
+      <c r="DC40" s="21"/>
+      <c r="DD40" s="21"/>
     </row>
-    <row r="41" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="13"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="15">
+    <row r="41" spans="2:108" ht="20" customHeight="1">
+      <c r="B41" s="18"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="20">
         <v>34174567</v>
       </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="17" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="N41" s="17" t="s">
+      <c r="N41" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="O41" s="16"/>
-      <c r="P41" s="15">
+      <c r="O41" s="21"/>
+      <c r="P41" s="20">
         <v>19240811</v>
       </c>
-      <c r="Q41" s="16"/>
-      <c r="R41" s="16"/>
-      <c r="S41" s="16"/>
-      <c r="T41" s="16"/>
-      <c r="U41" s="16"/>
-      <c r="V41" s="16"/>
-      <c r="W41" s="16"/>
-      <c r="X41" s="16"/>
-      <c r="Y41" s="16"/>
-      <c r="Z41" s="16"/>
-      <c r="AA41" s="16"/>
-      <c r="AB41" s="16"/>
-      <c r="AC41" s="16"/>
-      <c r="AD41" s="16"/>
-      <c r="AE41" s="16"/>
-      <c r="AF41" s="16"/>
-      <c r="AG41" s="16"/>
-      <c r="AH41" s="16"/>
-      <c r="AI41" s="16"/>
-      <c r="AJ41" s="16"/>
-      <c r="AK41" s="16"/>
-      <c r="AL41" s="16"/>
-      <c r="AM41" s="16"/>
-      <c r="AN41" s="16"/>
-      <c r="AO41" s="16"/>
-      <c r="AP41" s="15">
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="21"/>
+      <c r="V41" s="21"/>
+      <c r="W41" s="21"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="21"/>
+      <c r="Z41" s="21"/>
+      <c r="AA41" s="21"/>
+      <c r="AB41" s="21"/>
+      <c r="AC41" s="21"/>
+      <c r="AD41" s="21"/>
+      <c r="AE41" s="21"/>
+      <c r="AF41" s="21"/>
+      <c r="AG41" s="21"/>
+      <c r="AH41" s="21"/>
+      <c r="AI41" s="21"/>
+      <c r="AJ41" s="21"/>
+      <c r="AK41" s="21"/>
+      <c r="AL41" s="21"/>
+      <c r="AM41" s="21"/>
+      <c r="AN41" s="21"/>
+      <c r="AO41" s="21"/>
+      <c r="AP41" s="20">
         <v>20050214</v>
       </c>
-      <c r="AQ41" s="16"/>
-      <c r="AR41" s="17" t="s">
+      <c r="AQ41" s="21"/>
+      <c r="AR41" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="AS41" s="16"/>
-      <c r="AT41" s="16"/>
-      <c r="AU41" s="16"/>
-      <c r="AV41" s="16"/>
-      <c r="AW41" s="16"/>
-      <c r="AX41" s="17" t="s">
+      <c r="AS41" s="21"/>
+      <c r="AT41" s="21"/>
+      <c r="AU41" s="21"/>
+      <c r="AV41" s="21"/>
+      <c r="AW41" s="21"/>
+      <c r="AX41" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AY41" s="16"/>
-      <c r="AZ41" s="25">
+      <c r="AY41" s="21"/>
+      <c r="AZ41" s="26">
         <v>101001035000</v>
       </c>
-      <c r="BA41" s="16"/>
-      <c r="BB41" s="16"/>
-      <c r="BC41" s="16"/>
-      <c r="BD41" s="17" t="s">
+      <c r="BA41" s="21"/>
+      <c r="BB41" s="21"/>
+      <c r="BC41" s="21"/>
+      <c r="BD41" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="BE41" s="17" t="s">
+      <c r="BE41" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="BF41" s="16"/>
-      <c r="BG41" s="16"/>
-      <c r="BH41" s="16"/>
-      <c r="BI41" s="16"/>
-      <c r="BJ41" s="16"/>
-      <c r="BK41" s="16"/>
-      <c r="BL41" s="16"/>
-      <c r="BM41" s="16"/>
-      <c r="BN41" s="16"/>
-      <c r="BO41" s="16"/>
-      <c r="BP41" s="16"/>
-      <c r="BQ41" s="16"/>
-      <c r="BR41" s="16"/>
-      <c r="BS41" s="16"/>
-      <c r="BT41" s="16"/>
-      <c r="BU41" s="16"/>
-      <c r="BV41" s="16"/>
-      <c r="BW41" s="16"/>
-      <c r="BX41" s="16"/>
-      <c r="BY41" s="16"/>
-      <c r="BZ41" s="16"/>
-      <c r="CA41" s="16"/>
-      <c r="CB41" s="16"/>
-      <c r="CC41" s="16"/>
-      <c r="CD41" s="17" t="s">
+      <c r="BF41" s="21"/>
+      <c r="BG41" s="21"/>
+      <c r="BH41" s="21"/>
+      <c r="BI41" s="21"/>
+      <c r="BJ41" s="21"/>
+      <c r="BK41" s="21"/>
+      <c r="BL41" s="21"/>
+      <c r="BM41" s="21"/>
+      <c r="BN41" s="21"/>
+      <c r="BO41" s="21"/>
+      <c r="BP41" s="21"/>
+      <c r="BQ41" s="21"/>
+      <c r="BR41" s="21"/>
+      <c r="BS41" s="21"/>
+      <c r="BT41" s="21"/>
+      <c r="BU41" s="21"/>
+      <c r="BV41" s="21"/>
+      <c r="BW41" s="21"/>
+      <c r="BX41" s="21"/>
+      <c r="BY41" s="21"/>
+      <c r="BZ41" s="21"/>
+      <c r="CA41" s="21"/>
+      <c r="CB41" s="21"/>
+      <c r="CC41" s="21"/>
+      <c r="CD41" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="CE41" s="16"/>
-      <c r="CF41" s="17" t="s">
+      <c r="CE41" s="21"/>
+      <c r="CF41" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="CG41" s="16"/>
-      <c r="CH41" s="16"/>
-      <c r="CI41" s="16"/>
-      <c r="CJ41" s="17" t="s">
+      <c r="CG41" s="21"/>
+      <c r="CH41" s="21"/>
+      <c r="CI41" s="21"/>
+      <c r="CJ41" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="CK41" s="15">
+      <c r="CK41" s="20">
         <v>5</v>
       </c>
-      <c r="CL41" s="17" t="s">
+      <c r="CL41" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="CM41" s="16"/>
-      <c r="CN41" s="16"/>
-      <c r="CO41" s="16"/>
-      <c r="CP41" s="16"/>
-      <c r="CQ41" s="16"/>
-      <c r="CR41" s="16"/>
-      <c r="CS41" s="16"/>
-      <c r="CT41" s="15">
+      <c r="CM41" s="21"/>
+      <c r="CN41" s="21"/>
+      <c r="CO41" s="21"/>
+      <c r="CP41" s="21"/>
+      <c r="CQ41" s="21"/>
+      <c r="CR41" s="21"/>
+      <c r="CS41" s="21"/>
+      <c r="CT41" s="21">
         <v>1</v>
       </c>
-      <c r="CU41" s="17" t="s">
+      <c r="CU41" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="CV41" s="17" t="s">
+      <c r="CV41" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="CW41" s="17" t="s">
+      <c r="CW41" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="CX41" s="17" t="s">
+      <c r="CX41" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="CY41" s="15">
+      <c r="CY41" s="21">
         <v>14.7</v>
       </c>
-      <c r="CZ41" s="15">
+      <c r="CZ41" s="21">
         <v>14.7</v>
       </c>
-      <c r="DA41" s="15">
+      <c r="DA41" s="21">
         <v>0</v>
       </c>
-      <c r="DB41" s="17" t="s">
+      <c r="DB41" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="DC41" s="17" t="s">
+      <c r="DC41" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="DD41" s="17" t="s">
+      <c r="DD41" s="21" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="20">
+    <row r="42" spans="2:108" ht="20" customHeight="1">
+      <c r="B42" s="13"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="15">
         <v>45285678</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
-      <c r="L42" s="21"/>
-      <c r="M42" s="22" t="s">
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="N42" s="22" t="s">
+      <c r="N42" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="O42" s="21"/>
-      <c r="P42" s="20">
+      <c r="O42" s="16"/>
+      <c r="P42" s="15">
         <v>19890315</v>
       </c>
-      <c r="Q42" s="21"/>
-      <c r="R42" s="21"/>
-      <c r="S42" s="21"/>
-      <c r="T42" s="21"/>
-      <c r="U42" s="21"/>
-      <c r="V42" s="21"/>
-      <c r="W42" s="21"/>
-      <c r="X42" s="21"/>
-      <c r="Y42" s="21"/>
-      <c r="Z42" s="21"/>
-      <c r="AA42" s="21"/>
-      <c r="AB42" s="21"/>
-      <c r="AC42" s="21"/>
-      <c r="AD42" s="21"/>
-      <c r="AE42" s="21"/>
-      <c r="AF42" s="21"/>
-      <c r="AG42" s="21"/>
-      <c r="AH42" s="21"/>
-      <c r="AI42" s="21"/>
-      <c r="AJ42" s="21"/>
-      <c r="AK42" s="21"/>
-      <c r="AL42" s="21"/>
-      <c r="AM42" s="21"/>
-      <c r="AN42" s="21"/>
-      <c r="AO42" s="21"/>
-      <c r="AP42" s="20">
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="16"/>
+      <c r="V42" s="16"/>
+      <c r="W42" s="16"/>
+      <c r="X42" s="16"/>
+      <c r="Y42" s="16"/>
+      <c r="Z42" s="16"/>
+      <c r="AA42" s="16"/>
+      <c r="AB42" s="16"/>
+      <c r="AC42" s="16"/>
+      <c r="AD42" s="16"/>
+      <c r="AE42" s="16"/>
+      <c r="AF42" s="16"/>
+      <c r="AG42" s="16"/>
+      <c r="AH42" s="16"/>
+      <c r="AI42" s="16"/>
+      <c r="AJ42" s="16"/>
+      <c r="AK42" s="16"/>
+      <c r="AL42" s="16"/>
+      <c r="AM42" s="16"/>
+      <c r="AN42" s="16"/>
+      <c r="AO42" s="16"/>
+      <c r="AP42" s="15">
         <v>20150702</v>
       </c>
-      <c r="AQ42" s="21"/>
-      <c r="AR42" s="22" t="s">
+      <c r="AQ42" s="16"/>
+      <c r="AR42" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AS42" s="21"/>
-      <c r="AT42" s="21"/>
-      <c r="AU42" s="21"/>
-      <c r="AV42" s="21"/>
-      <c r="AW42" s="21"/>
-      <c r="AX42" s="22" t="s">
+      <c r="AS42" s="16"/>
+      <c r="AT42" s="16"/>
+      <c r="AU42" s="16"/>
+      <c r="AV42" s="16"/>
+      <c r="AW42" s="16"/>
+      <c r="AX42" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="AY42" s="21"/>
-      <c r="AZ42" s="26">
+      <c r="AY42" s="16"/>
+      <c r="AZ42" s="25">
         <v>101001055000</v>
       </c>
-      <c r="BA42" s="21"/>
-      <c r="BB42" s="21"/>
-      <c r="BC42" s="21"/>
-      <c r="BD42" s="22" t="s">
+      <c r="BA42" s="16"/>
+      <c r="BB42" s="16"/>
+      <c r="BC42" s="16"/>
+      <c r="BD42" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="BE42" s="22" t="s">
+      <c r="BE42" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="BF42" s="21"/>
-      <c r="BG42" s="21"/>
-      <c r="BH42" s="21"/>
-      <c r="BI42" s="21"/>
-      <c r="BJ42" s="21"/>
-      <c r="BK42" s="21"/>
-      <c r="BL42" s="21"/>
-      <c r="BM42" s="21"/>
-      <c r="BN42" s="21"/>
-      <c r="BO42" s="21"/>
-      <c r="BP42" s="21"/>
-      <c r="BQ42" s="21"/>
-      <c r="BR42" s="21"/>
-      <c r="BS42" s="21"/>
-      <c r="BT42" s="21"/>
-      <c r="BU42" s="21"/>
-      <c r="BV42" s="21"/>
-      <c r="BW42" s="21"/>
-      <c r="BX42" s="21"/>
-      <c r="BY42" s="21"/>
-      <c r="BZ42" s="21"/>
-      <c r="CA42" s="21"/>
-      <c r="CB42" s="21"/>
-      <c r="CC42" s="21"/>
-      <c r="CD42" s="22" t="s">
+      <c r="BF42" s="16"/>
+      <c r="BG42" s="16"/>
+      <c r="BH42" s="16"/>
+      <c r="BI42" s="16"/>
+      <c r="BJ42" s="16"/>
+      <c r="BK42" s="16"/>
+      <c r="BL42" s="16"/>
+      <c r="BM42" s="16"/>
+      <c r="BN42" s="16"/>
+      <c r="BO42" s="16"/>
+      <c r="BP42" s="16"/>
+      <c r="BQ42" s="16"/>
+      <c r="BR42" s="16"/>
+      <c r="BS42" s="16"/>
+      <c r="BT42" s="16"/>
+      <c r="BU42" s="16"/>
+      <c r="BV42" s="16"/>
+      <c r="BW42" s="16"/>
+      <c r="BX42" s="16"/>
+      <c r="BY42" s="16"/>
+      <c r="BZ42" s="16"/>
+      <c r="CA42" s="16"/>
+      <c r="CB42" s="16"/>
+      <c r="CC42" s="16"/>
+      <c r="CD42" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="CE42" s="21"/>
-      <c r="CF42" s="22" t="s">
+      <c r="CE42" s="16"/>
+      <c r="CF42" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="CG42" s="21"/>
-      <c r="CH42" s="21"/>
-      <c r="CI42" s="21"/>
-      <c r="CJ42" s="22" t="s">
+      <c r="CG42" s="16"/>
+      <c r="CH42" s="16"/>
+      <c r="CI42" s="16"/>
+      <c r="CJ42" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="CK42" s="20">
+      <c r="CK42" s="16">
         <v>6</v>
       </c>
-      <c r="CL42" s="22" t="s">
+      <c r="CL42" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="CM42" s="21"/>
-      <c r="CN42" s="21"/>
-      <c r="CO42" s="21"/>
-      <c r="CP42" s="21"/>
-      <c r="CQ42" s="21"/>
-      <c r="CR42" s="21"/>
-      <c r="CS42" s="21"/>
-      <c r="CT42" s="21"/>
-      <c r="CU42" s="21"/>
-      <c r="CV42" s="21"/>
-      <c r="CW42" s="21"/>
-      <c r="CX42" s="21"/>
-      <c r="CY42" s="21"/>
-      <c r="CZ42" s="21"/>
-      <c r="DA42" s="21"/>
-      <c r="DB42" s="21"/>
-      <c r="DC42" s="21"/>
-      <c r="DD42" s="21"/>
+      <c r="CM42" s="16"/>
+      <c r="CN42" s="16"/>
+      <c r="CO42" s="16"/>
+      <c r="CP42" s="16"/>
+      <c r="CQ42" s="16"/>
+      <c r="CR42" s="16"/>
+      <c r="CS42" s="16"/>
+      <c r="CT42" s="16"/>
+      <c r="CU42" s="16"/>
+      <c r="CV42" s="16"/>
+      <c r="CW42" s="16"/>
+      <c r="CX42" s="16"/>
+      <c r="CY42" s="16"/>
+      <c r="CZ42" s="16"/>
+      <c r="DA42" s="16"/>
+      <c r="DB42" s="16"/>
+      <c r="DC42" s="16"/>
+      <c r="DD42" s="16"/>
     </row>
-    <row r="43" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20">
+    <row r="43" spans="2:108" ht="20" customHeight="1">
+      <c r="B43" s="13"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="15">
         <v>45285678</v>
       </c>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="21"/>
-      <c r="M43" s="22" t="s">
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="N43" s="22" t="s">
+      <c r="N43" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="O43" s="21"/>
-      <c r="P43" s="20">
+      <c r="O43" s="16"/>
+      <c r="P43" s="15">
         <v>19890315</v>
       </c>
-      <c r="Q43" s="21"/>
-      <c r="R43" s="21"/>
-      <c r="S43" s="21"/>
-      <c r="T43" s="21"/>
-      <c r="U43" s="21"/>
-      <c r="V43" s="21"/>
-      <c r="W43" s="21"/>
-      <c r="X43" s="21"/>
-      <c r="Y43" s="21"/>
-      <c r="Z43" s="21"/>
-      <c r="AA43" s="21"/>
-      <c r="AB43" s="21"/>
-      <c r="AC43" s="21"/>
-      <c r="AD43" s="21"/>
-      <c r="AE43" s="21"/>
-      <c r="AF43" s="21"/>
-      <c r="AG43" s="21"/>
-      <c r="AH43" s="21"/>
-      <c r="AI43" s="21"/>
-      <c r="AJ43" s="21"/>
-      <c r="AK43" s="21"/>
-      <c r="AL43" s="21"/>
-      <c r="AM43" s="21"/>
-      <c r="AN43" s="21"/>
-      <c r="AO43" s="21"/>
-      <c r="AP43" s="20">
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="16"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="16"/>
+      <c r="W43" s="16"/>
+      <c r="X43" s="16"/>
+      <c r="Y43" s="16"/>
+      <c r="Z43" s="16"/>
+      <c r="AA43" s="16"/>
+      <c r="AB43" s="16"/>
+      <c r="AC43" s="16"/>
+      <c r="AD43" s="16"/>
+      <c r="AE43" s="16"/>
+      <c r="AF43" s="16"/>
+      <c r="AG43" s="16"/>
+      <c r="AH43" s="16"/>
+      <c r="AI43" s="16"/>
+      <c r="AJ43" s="16"/>
+      <c r="AK43" s="16"/>
+      <c r="AL43" s="16"/>
+      <c r="AM43" s="16"/>
+      <c r="AN43" s="16"/>
+      <c r="AO43" s="16"/>
+      <c r="AP43" s="15">
         <v>20000702</v>
       </c>
-      <c r="AQ43" s="21"/>
-      <c r="AR43" s="22" t="s">
+      <c r="AQ43" s="16"/>
+      <c r="AR43" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AS43" s="21"/>
-      <c r="AT43" s="21"/>
-      <c r="AU43" s="21"/>
-      <c r="AV43" s="21"/>
-      <c r="AW43" s="21"/>
-      <c r="AX43" s="22" t="s">
+      <c r="AS43" s="16"/>
+      <c r="AT43" s="16"/>
+      <c r="AU43" s="16"/>
+      <c r="AV43" s="16"/>
+      <c r="AW43" s="16"/>
+      <c r="AX43" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="AY43" s="21"/>
-      <c r="AZ43" s="26">
+      <c r="AY43" s="16"/>
+      <c r="AZ43" s="25">
         <v>102001056000</v>
       </c>
-      <c r="BA43" s="21"/>
-      <c r="BB43" s="21"/>
-      <c r="BC43" s="21"/>
-      <c r="BD43" s="22" t="s">
+      <c r="BA43" s="16"/>
+      <c r="BB43" s="16"/>
+      <c r="BC43" s="16"/>
+      <c r="BD43" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="BE43" s="22" t="s">
+      <c r="BE43" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="BF43" s="21"/>
-      <c r="BG43" s="21"/>
-      <c r="BH43" s="21"/>
-      <c r="BI43" s="21"/>
-      <c r="BJ43" s="21"/>
-      <c r="BK43" s="21"/>
-      <c r="BL43" s="21"/>
-      <c r="BM43" s="21"/>
-      <c r="BN43" s="21"/>
-      <c r="BO43" s="21"/>
-      <c r="BP43" s="21"/>
-      <c r="BQ43" s="21"/>
-      <c r="BR43" s="21"/>
-      <c r="BS43" s="21"/>
-      <c r="BT43" s="21"/>
-      <c r="BU43" s="21"/>
-      <c r="BV43" s="21"/>
-      <c r="BW43" s="21"/>
-      <c r="BX43" s="21"/>
-      <c r="BY43" s="21"/>
-      <c r="BZ43" s="21"/>
-      <c r="CA43" s="21"/>
-      <c r="CB43" s="21"/>
-      <c r="CC43" s="21"/>
-      <c r="CD43" s="22" t="s">
+      <c r="BF43" s="16"/>
+      <c r="BG43" s="16"/>
+      <c r="BH43" s="16"/>
+      <c r="BI43" s="16"/>
+      <c r="BJ43" s="16"/>
+      <c r="BK43" s="16"/>
+      <c r="BL43" s="16"/>
+      <c r="BM43" s="16"/>
+      <c r="BN43" s="16"/>
+      <c r="BO43" s="16"/>
+      <c r="BP43" s="16"/>
+      <c r="BQ43" s="16"/>
+      <c r="BR43" s="16"/>
+      <c r="BS43" s="16"/>
+      <c r="BT43" s="16"/>
+      <c r="BU43" s="16"/>
+      <c r="BV43" s="16"/>
+      <c r="BW43" s="16"/>
+      <c r="BX43" s="16"/>
+      <c r="BY43" s="16"/>
+      <c r="BZ43" s="16"/>
+      <c r="CA43" s="16"/>
+      <c r="CB43" s="16"/>
+      <c r="CC43" s="16"/>
+      <c r="CD43" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="CE43" s="21"/>
-      <c r="CF43" s="22" t="s">
+      <c r="CE43" s="16"/>
+      <c r="CF43" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="CG43" s="21"/>
-      <c r="CH43" s="21"/>
-      <c r="CI43" s="21"/>
-      <c r="CJ43" s="22" t="s">
+      <c r="CG43" s="16"/>
+      <c r="CH43" s="16"/>
+      <c r="CI43" s="16"/>
+      <c r="CJ43" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="CK43" s="20">
+      <c r="CK43" s="16">
         <v>6</v>
       </c>
-      <c r="CL43" s="22" t="s">
+      <c r="CL43" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="CM43" s="21"/>
-      <c r="CN43" s="21"/>
-      <c r="CO43" s="21"/>
-      <c r="CP43" s="21"/>
-      <c r="CQ43" s="21"/>
-      <c r="CR43" s="21"/>
-      <c r="CS43" s="21"/>
-      <c r="CT43" s="20">
+      <c r="CM43" s="16"/>
+      <c r="CN43" s="16"/>
+      <c r="CO43" s="16"/>
+      <c r="CP43" s="16"/>
+      <c r="CQ43" s="16"/>
+      <c r="CR43" s="16"/>
+      <c r="CS43" s="16"/>
+      <c r="CT43" s="16">
         <v>2</v>
       </c>
-      <c r="CU43" s="22" t="s">
+      <c r="CU43" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="CV43" s="22" t="s">
+      <c r="CV43" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="CW43" s="22" t="s">
+      <c r="CW43" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="CX43" s="22" t="s">
+      <c r="CX43" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="CY43" s="20">
+      <c r="CY43" s="16">
         <v>19.399999999999999</v>
       </c>
-      <c r="CZ43" s="20">
+      <c r="CZ43" s="16">
         <v>4.4000000000000004</v>
       </c>
-      <c r="DA43" s="20">
+      <c r="DA43" s="16">
         <v>1</v>
       </c>
-      <c r="DB43" s="22" t="s">
+      <c r="DB43" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="DC43" s="22" t="s">
+      <c r="DC43" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="DD43" s="22" t="s">
+      <c r="DD43" s="16" t="s">
         <v>167</v>
       </c>
     </row>
@@ -8931,5 +8935,10 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>